<commit_message>
Changed UI elements & some Documents & added Highscore class UI changes: Launcher Symbol, Tower Icons, Map
</commit_message>
<xml_diff>
--- a/svn/JG16S17P06/trunk/Documentation/ProjectDocumentation/Website_template.xlsx
+++ b/svn/JG16S17P06/trunk/Documentation/ProjectDocumentation/Website_template.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bernhard\StudioProjects\ElementTD\svn\JG16S17P06\trunk\Documentation\ProjectDocumentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="15" windowWidth="19320" windowHeight="14520"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Titel</t>
   </si>
@@ -78,9 +83,6 @@
     <t>Freigabe</t>
   </si>
   <si>
-    <t>Martina Musterfrau, Max Mustermann</t>
-  </si>
-  <si>
     <t>FH-Studenten</t>
   </si>
   <si>
@@ -96,24 +98,12 @@
     <t>Vollständiger Titel und Name des Projektbetreuers</t>
   </si>
   <si>
-    <t>Musterfirma</t>
-  </si>
-  <si>
     <t>Hier soll eine Kurzbeschreibung des Projekts eingefügt werden. Dieser Kurztext wird neben dem Logo des Projekts (1. Bild) auf der Projektübersichtsseite zu lesen sein. Die Länge sollte ca. 2-3 Sätze betragen.</t>
   </si>
   <si>
-    <t>Mustertitel</t>
-  </si>
-  <si>
-    <t>DI Dr. Max Mustermann, BSc, MSc</t>
-  </si>
-  <si>
     <t>Liste der Namen der Studierenden, die an diesem Projekt mitarbeiten, mit Komma getrennt.</t>
   </si>
   <si>
-    <t>Bild1.jpg,Bild2.png,Bild3.gif</t>
-  </si>
-  <si>
     <t>Ausfüllhinweise: Für 1 Projekt muss jeweils 1 Zeile ausgefüllt werden. Zu verwenden ist die obige Zeile mit den Musterdaten. Die ausgeblendeten Spalten sollen nicht eingeblendet werden.</t>
   </si>
   <si>
@@ -132,24 +122,32 @@
     <t>Bei Unklarheiten können die aktuellen Projektbeschreibungen auf der Website als Referenz herangezogen werden. Bei konkreten Fragen ist Kontakt mit Stephan Drab aufzunehmen.</t>
   </si>
   <si>
-    <t>Dies ist der Musterlangtext. Dies ist der Musterlangtext. Dies ist der Musterlangtext. Dies ist der Musterlangtext. Dies ist der Musterlangtext.
-Dies ist der Musterlangtext. Dies ist der Musterlangtext. Dies ist der Musterlangtext. Dies ist der Musterlangtext. Dies ist der Musterlangtext. Dies ist der Musterlangtext.</t>
-  </si>
-  <si>
-    <t>Dies ist eine Musterkurzbeschreibung. Dies ist eine Musterkurzbeschreibung.</t>
-  </si>
-  <si>
-    <t>Sommersemester 2009</t>
-  </si>
-  <si>
     <t>abgeschlossen</t>
+  </si>
+  <si>
+    <t>ElementTD</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>Sommersemester 2017</t>
+  </si>
+  <si>
+    <t>GEBAUER Laurenz, PRANZ Bernhard, SCHILLER Markus</t>
+  </si>
+  <si>
+    <t>MACHEINER Martin, BSc</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -298,15 +296,23 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -348,7 +354,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -380,9 +386,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -414,6 +438,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -589,14 +631,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
@@ -620,7 +662,7 @@
     <col min="20" max="20" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="5" customFormat="1">
+    <row r="1" spans="1:20" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -682,50 +724,53 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="6" customFormat="1" ht="12.75" customHeight="1">
+    <row r="2" spans="1:20" s="6" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D2" s="6">
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H2" s="6">
         <v>0</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>39</v>
       </c>
       <c r="T2" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:20" s="6" customFormat="1"/>
-    <row r="4" spans="1:20" s="6" customFormat="1"/>
-    <row r="5" spans="1:20" s="6" customFormat="1"/>
-    <row r="6" spans="1:20">
+    <row r="3" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
@@ -742,12 +787,12 @@
       <c r="N6" s="11"/>
       <c r="O6" s="11"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
@@ -763,12 +808,12 @@
       <c r="N7" s="11"/>
       <c r="O7" s="11"/>
     </row>
-    <row r="8" spans="1:20" ht="52.5" customHeight="1">
+    <row r="8" spans="1:20" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
@@ -784,12 +829,12 @@
       <c r="N8" s="11"/>
       <c r="O8" s="11"/>
     </row>
-    <row r="9" spans="1:20" ht="27.75" customHeight="1">
+    <row r="9" spans="1:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" s="11"/>
       <c r="D9" s="11"/>
@@ -805,12 +850,12 @@
       <c r="N9" s="11"/>
       <c r="O9" s="11"/>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
@@ -826,12 +871,12 @@
       <c r="N10" s="13"/>
       <c r="O10" s="14"/>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
@@ -847,12 +892,12 @@
       <c r="N11" s="11"/>
       <c r="O11" s="11"/>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -868,12 +913,12 @@
       <c r="N12" s="11"/>
       <c r="O12" s="11"/>
     </row>
-    <row r="13" spans="1:20" ht="39" customHeight="1">
+    <row r="13" spans="1:20" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -889,9 +934,9 @@
       <c r="N13" s="15"/>
       <c r="O13" s="15"/>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -929,12 +974,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>
@@ -943,12 +988,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.4921259845" footer="0.4921259845"/>

</xml_diff>

<commit_message>
changed Tiles and some Documents
</commit_message>
<xml_diff>
--- a/svn/JG16S17P06/trunk/Documentation/ProjectDocumentation/Website_template.xlsx
+++ b/svn/JG16S17P06/trunk/Documentation/ProjectDocumentation/Website_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>Titel</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Ein Tower-Defense-Spiel, bei dem es das Ziel ist, Gruppen von herankommenden Gegnern zu eliminieren. Hierfür werden Türme aus Elementen gebaut, die miteinander fusioniert werden können.</t>
+  </si>
+  <si>
+    <t>Ziel des Projekts ist die Implementierung eines plattformübergreifenden Tower-Defense-Spiels, bei dem Mithilfe elementarer Kombinationen aus verschiedensten Ele-menten Türme gebaut werden können. Hierbei gibt es fixe vordefinierte Elemente: Feu-er, Wasser, Stein, Natur, Dunkelheit, Licht. Diese daraus entstandenen Türme sollen feindliche Nicht-Spieler-Charakter (NPCs), welche gruppenweise erscheinen, daran hindern, die Karte zu überqueren. Auf dieser ist eine vordefinierte Route, welche als Einbahn aufgebaut ist, auf der die Gegner die Karte von Punkt A zu Punkt B durchlau-fen. Am Rande dieser Route kann der Benutzer die vorher erwähnten Türme platzieren und so die NPCs daran hindern die Karte zu überqueren. Wenn eine gewisse Anzahl an NPCs die Karte erfolgreich überquert hat, hat der Spieler verloren.</t>
   </si>
 </sst>
 </file>
@@ -635,7 +641,7 @@
   <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -741,7 +747,7 @@
         <v>33</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H2" s="6">
         <v>0</v>
@@ -756,7 +762,7 @@
         <v>39</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="S2" s="6" t="s">
         <v>39</v>

</xml_diff>